<commit_message>
:bug: Fixed a bug in the video editing script to improve the accuracy of the magenta detecting algorithm.
</commit_message>
<xml_diff>
--- a/Documentation/Video Recording Progress.xlsx
+++ b/Documentation/Video Recording Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fcortevargas/Thesis/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BD5A5F-5144-AE40-B58F-7FCF9CF27B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6F9B90-0930-014E-A062-B00B13420B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1780" windowWidth="28040" windowHeight="17440" xr2:uid="{E3E76E12-45DE-2C46-8A4D-60502D85C9C5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E3E76E12-45DE-2C46-8A4D-60502D85C9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>From</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Side View Individuals Edited</t>
+  </si>
+  <si>
+    <t>Side View Individuals Uploaded to Webdrive</t>
+  </si>
+  <si>
+    <t>Top View Individuals Uploaded to Webdrive</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -151,16 +157,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -201,6 +197,56 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -534,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85946DCC-AE16-1745-9D48-0F96638A2D30}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -551,10 +597,12 @@
     <col min="7" max="7" width="43.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="38" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="58" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="58.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
@@ -579,8 +627,14 @@
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -608,8 +662,14 @@
       <c r="I2" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -637,8 +697,14 @@
       <c r="I3" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -666,8 +732,14 @@
       <c r="I4" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -695,8 +767,14 @@
       <c r="I5" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -724,8 +802,14 @@
       <c r="I6" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -753,8 +837,14 @@
       <c r="I7" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -782,8 +872,14 @@
       <c r="I8" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -811,8 +907,14 @@
       <c r="I9" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -838,10 +940,16 @@
         <v>0</v>
       </c>
       <c r="I10" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -867,10 +975,16 @@
         <v>0</v>
       </c>
       <c r="I11" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -896,10 +1010,16 @@
         <v>0</v>
       </c>
       <c r="I12" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -925,10 +1045,16 @@
         <v>0</v>
       </c>
       <c r="I13" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -956,8 +1082,14 @@
       <c r="I14" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -985,8 +1117,14 @@
       <c r="I15" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1014,8 +1152,14 @@
       <c r="I16" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1043,8 +1187,14 @@
       <c r="I17" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1072,8 +1222,14 @@
       <c r="I18" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1101,8 +1257,14 @@
       <c r="I19" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1130,8 +1292,14 @@
       <c r="I20" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1159,8 +1327,14 @@
       <c r="I21" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1188,8 +1362,14 @@
       <c r="I22" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1217,8 +1397,14 @@
       <c r="I23" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1246,8 +1432,14 @@
       <c r="I24" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1275,8 +1467,14 @@
       <c r="I25" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1304,8 +1502,14 @@
       <c r="I26" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -1333,8 +1537,14 @@
       <c r="I27" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1362,8 +1572,14 @@
       <c r="I28" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -1391,8 +1607,14 @@
       <c r="I29" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1420,8 +1642,14 @@
       <c r="I30" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1449,8 +1677,14 @@
       <c r="I31" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -1478,8 +1712,14 @@
       <c r="I32" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -1507,30 +1747,52 @@
       <c r="I33" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E33">
-    <cfRule type="containsText" dxfId="5" priority="14" operator="containsText" text="False">
+    <cfRule type="containsText" dxfId="9" priority="17" operator="containsText" text="True">
+      <formula>NOT(ISERROR(SEARCH("True",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="18" operator="containsText" text="False">
       <formula>NOT(ISERROR(SEARCH("False",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="13" operator="containsText" text="True">
-      <formula>NOT(ISERROR(SEARCH("True",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F40">
-    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="False">
+    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="True">
+      <formula>NOT(ISERROR(SEARCH("True",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="False">
       <formula>NOT(ISERROR(SEARCH("False",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="True">
-      <formula>NOT(ISERROR(SEARCH("True",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:I33">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="True">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="True">
       <formula>NOT(ISERROR(SEARCH("True",G2)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="False">
+      <formula>NOT(ISERROR(SEARCH("False",G2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13:K33 J2:J12">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="True">
+      <formula>NOT(ISERROR(SEARCH("True",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="False">
+      <formula>NOT(ISERROR(SEARCH("False",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K12">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="True">
+      <formula>NOT(ISERROR(SEARCH("True",K2)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="False">
-      <formula>NOT(ISERROR(SEARCH("False",G2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("False",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
:memo: Updated video progress log.
</commit_message>
<xml_diff>
--- a/Documentation/Video Recording Progress.xlsx
+++ b/Documentation/Video Recording Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fcortevargas/Thesis/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6F9B90-0930-014E-A062-B00B13420B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A864ADD-0203-DD4D-B3C8-91ED91E0F669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E3E76E12-45DE-2C46-8A4D-60502D85C9C5}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{E3E76E12-45DE-2C46-8A4D-60502D85C9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>From</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Top View Individuals Uploaded to Webdrive</t>
+  </si>
+  <si>
+    <t>Examples</t>
   </si>
 </sst>
 </file>
@@ -126,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -145,31 +148,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -580,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85946DCC-AE16-1745-9D48-0F96638A2D30}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -594,11 +580,11 @@
     <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="43.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="37.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="38" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="58" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="58.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="58.6640625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -654,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1" t="b">
         <v>0</v>
@@ -666,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -689,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1" t="b">
         <v>0</v>
@@ -701,7 +687,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -724,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1" t="b">
         <v>0</v>
@@ -736,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -759,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1" t="b">
         <v>0</v>
@@ -771,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -794,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1" t="b">
         <v>0</v>
@@ -806,7 +792,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -829,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="b">
         <v>0</v>
@@ -841,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -864,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1" t="b">
         <v>0</v>
@@ -876,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1080,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="1" t="b">
         <v>0</v>
@@ -1115,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="1" t="b">
         <v>0</v>
@@ -1150,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="1" t="b">
         <v>0</v>
@@ -1185,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="1" t="b">
         <v>0</v>
@@ -1220,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="1" t="b">
         <v>0</v>
@@ -1255,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="1" t="b">
         <v>0</v>
@@ -1290,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="1" t="b">
         <v>0</v>
@@ -1325,7 +1311,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="1" t="b">
         <v>0</v>
@@ -1360,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="1" t="b">
         <v>0</v>
@@ -1395,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="1" t="b">
         <v>0</v>
@@ -1430,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="1" t="b">
         <v>0</v>
@@ -1465,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="1" t="b">
         <v>0</v>
@@ -1500,7 +1486,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="1" t="b">
         <v>0</v>
@@ -1529,13 +1515,13 @@
         <v>0</v>
       </c>
       <c r="G27" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I27" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" s="1" t="b">
         <v>0</v>
@@ -1564,13 +1550,13 @@
         <v>0</v>
       </c>
       <c r="G28" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I28" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="1" t="b">
         <v>0</v>
@@ -1599,13 +1585,13 @@
         <v>0</v>
       </c>
       <c r="G29" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I29" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="1" t="b">
         <v>0</v>
@@ -1634,13 +1620,13 @@
         <v>0</v>
       </c>
       <c r="G30" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I30" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="1" t="b">
         <v>0</v>
@@ -1669,13 +1655,13 @@
         <v>0</v>
       </c>
       <c r="G31" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I31" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" s="1" t="b">
         <v>0</v>
@@ -1695,10 +1681,10 @@
         <v>496</v>
       </c>
       <c r="D32" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="1" t="b">
         <v>0</v>
@@ -1730,10 +1716,10 @@
         <v>512</v>
       </c>
       <c r="D33" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="1" t="b">
         <v>0</v>
@@ -1754,45 +1740,73 @@
         <v>0</v>
       </c>
     </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:E33">
-    <cfRule type="containsText" dxfId="9" priority="17" operator="containsText" text="True">
+  <mergeCells count="1">
+    <mergeCell ref="B34:C34"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D2:E33 G2:K8">
+    <cfRule type="containsText" dxfId="7" priority="23" operator="containsText" text="True">
       <formula>NOT(ISERROR(SEARCH("True",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="18" operator="containsText" text="False">
+    <cfRule type="containsText" dxfId="6" priority="24" operator="containsText" text="False">
       <formula>NOT(ISERROR(SEARCH("False",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F40">
-    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="True">
+    <cfRule type="containsText" dxfId="5" priority="21" operator="containsText" text="True">
       <formula>NOT(ISERROR(SEARCH("True",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="False">
+    <cfRule type="containsText" dxfId="4" priority="22" operator="containsText" text="False">
       <formula>NOT(ISERROR(SEARCH("False",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:I33">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="True">
-      <formula>NOT(ISERROR(SEARCH("True",G2)))</formula>
+  <conditionalFormatting sqref="G34:H34 J34:K34 G9:K33">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="True">
+      <formula>NOT(ISERROR(SEARCH("True",G9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="False">
-      <formula>NOT(ISERROR(SEARCH("False",G2)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="False">
+      <formula>NOT(ISERROR(SEARCH("False",G9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13:K33 J2:J12">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="True">
-      <formula>NOT(ISERROR(SEARCH("True",J2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="False">
-      <formula>NOT(ISERROR(SEARCH("False",J2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K12">
+  <conditionalFormatting sqref="D34:E34 I34">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="True">
-      <formula>NOT(ISERROR(SEARCH("True",K2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("True",D34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="False">
-      <formula>NOT(ISERROR(SEARCH("False",K2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("False",D34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
:memo: Updated video recording progress log.
</commit_message>
<xml_diff>
--- a/Documentation/Video Recording Progress.xlsx
+++ b/Documentation/Video Recording Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fcortevargas/Thesis/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A864ADD-0203-DD4D-B3C8-91ED91E0F669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E99061-B2F8-CB43-8644-7DD45FFA0AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{E3E76E12-45DE-2C46-8A4D-60502D85C9C5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{E3E76E12-45DE-2C46-8A4D-60502D85C9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,47 +155,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -569,23 +529,25 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H1" sqref="H1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="43" style="1" customWidth="1"/>
     <col min="7" max="7" width="43.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="37.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="38" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="58" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="38" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="58" style="1" customWidth="1"/>
     <col min="11" max="11" width="58.6640625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="12" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="10.83203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -643,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1" t="b">
         <v>1</v>
@@ -678,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1" t="b">
         <v>1</v>
@@ -713,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1" t="b">
         <v>1</v>
@@ -748,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1" t="b">
         <v>1</v>
@@ -783,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1" t="b">
         <v>1</v>
@@ -818,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="b">
         <v>1</v>
@@ -853,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1" t="b">
         <v>1</v>
@@ -888,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1" t="b">
         <v>1</v>
@@ -923,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1" t="b">
         <v>1</v>
@@ -958,7 +920,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1" t="b">
         <v>1</v>
@@ -993,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1" t="b">
         <v>1</v>
@@ -1028,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1" t="b">
         <v>1</v>
@@ -1063,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1" t="b">
         <v>1</v>
@@ -1098,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1" t="b">
         <v>1</v>
@@ -1133,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="1" t="b">
         <v>1</v>
@@ -1168,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="1" t="b">
         <v>1</v>
@@ -1203,7 +1165,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="1" t="b">
         <v>1</v>
@@ -1238,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="1" t="b">
         <v>1</v>
@@ -1273,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="1" t="b">
         <v>1</v>
@@ -1308,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="1" t="b">
         <v>1</v>
@@ -1343,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="1" t="b">
         <v>1</v>
@@ -1378,7 +1340,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1" t="b">
         <v>1</v>
@@ -1413,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="1" t="b">
         <v>1</v>
@@ -1448,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="1" t="b">
         <v>1</v>
@@ -1483,7 +1445,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="1" t="b">
         <v>1</v>
@@ -1518,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="1" t="b">
         <v>1</v>
@@ -1553,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="1" t="b">
         <v>1</v>
@@ -1588,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="1" t="b">
         <v>1</v>
@@ -1623,7 +1585,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="1" t="b">
         <v>1</v>
@@ -1658,7 +1620,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="1" t="b">
         <v>1</v>
@@ -1693,10 +1655,10 @@
         <v>0</v>
       </c>
       <c r="H32" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" s="1" t="b">
         <v>0</v>
@@ -1728,10 +1690,10 @@
         <v>0</v>
       </c>
       <c r="H33" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" s="1" t="b">
         <v>0</v>
@@ -1761,10 +1723,10 @@
         <v>0</v>
       </c>
       <c r="H34" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" s="1" t="b">
         <v>0</v>
@@ -1777,36 +1739,20 @@
   <mergeCells count="1">
     <mergeCell ref="B34:C34"/>
   </mergeCells>
-  <conditionalFormatting sqref="D2:E33 G2:K8">
-    <cfRule type="containsText" dxfId="7" priority="23" operator="containsText" text="True">
+  <conditionalFormatting sqref="D2:E34 G2:K34">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="True">
       <formula>NOT(ISERROR(SEARCH("True",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="24" operator="containsText" text="False">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="False">
       <formula>NOT(ISERROR(SEARCH("False",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F40">
-    <cfRule type="containsText" dxfId="5" priority="21" operator="containsText" text="True">
+    <cfRule type="containsText" dxfId="1" priority="21" operator="containsText" text="True">
       <formula>NOT(ISERROR(SEARCH("True",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="22" operator="containsText" text="False">
+    <cfRule type="containsText" dxfId="0" priority="22" operator="containsText" text="False">
       <formula>NOT(ISERROR(SEARCH("False",F2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34:H34 J34:K34 G9:K33">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="True">
-      <formula>NOT(ISERROR(SEARCH("True",G9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="False">
-      <formula>NOT(ISERROR(SEARCH("False",G9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34:E34 I34">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="True">
-      <formula>NOT(ISERROR(SEARCH("True",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="False">
-      <formula>NOT(ISERROR(SEARCH("False",D34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
:fire: Deleted an unnecessary file.
</commit_message>
<xml_diff>
--- a/Documentation/Video Recording Progress.xlsx
+++ b/Documentation/Video Recording Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fcortevargas/Thesis/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F53395-8138-4942-A66F-7CD71AED116B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A49AA9-03B4-4640-9440-5ECD27B63B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{E3E76E12-45DE-2C46-8A4D-60502D85C9C5}"/>
   </bookViews>
@@ -1933,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95367985-2CDA-8742-AA4C-0FF0C0A9DC04}">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A479" workbookViewId="0">
-      <selection activeCell="C479" sqref="C479"/>
+    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
+      <selection activeCell="C479" sqref="C479:H513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14388,19 +14388,19 @@
         <v>1</v>
       </c>
       <c r="D479" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E479" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F479" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G479" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H479" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="480" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14414,19 +14414,19 @@
         <v>1</v>
       </c>
       <c r="D480" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E480" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F480" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G480" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H480" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="481" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14440,19 +14440,19 @@
         <v>1</v>
       </c>
       <c r="D481" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E481" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F481" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G481" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H481" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="482" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14466,19 +14466,19 @@
         <v>1</v>
       </c>
       <c r="D482" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E482" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F482" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G482" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H482" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="483" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14492,19 +14492,19 @@
         <v>1</v>
       </c>
       <c r="D483" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E483" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F483" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G483" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H483" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="484" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14518,19 +14518,19 @@
         <v>1</v>
       </c>
       <c r="D484" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E484" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F484" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G484" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H484" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="485" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14544,19 +14544,19 @@
         <v>1</v>
       </c>
       <c r="D485" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E485" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F485" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G485" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H485" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="486" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14570,19 +14570,19 @@
         <v>1</v>
       </c>
       <c r="D486" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E486" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F486" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G486" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H486" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="487" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14596,19 +14596,19 @@
         <v>1</v>
       </c>
       <c r="D487" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E487" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F487" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G487" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H487" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="488" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14622,19 +14622,19 @@
         <v>1</v>
       </c>
       <c r="D488" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E488" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F488" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G488" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H488" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="489" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14648,19 +14648,19 @@
         <v>1</v>
       </c>
       <c r="D489" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E489" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F489" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G489" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H489" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="490" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14674,19 +14674,19 @@
         <v>1</v>
       </c>
       <c r="D490" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E490" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F490" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G490" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H490" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="491" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14700,19 +14700,19 @@
         <v>1</v>
       </c>
       <c r="D491" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E491" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F491" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G491" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H491" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="492" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14726,19 +14726,19 @@
         <v>1</v>
       </c>
       <c r="D492" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E492" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F492" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G492" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H492" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="493" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14752,19 +14752,19 @@
         <v>1</v>
       </c>
       <c r="D493" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E493" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F493" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G493" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H493" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="494" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14778,19 +14778,19 @@
         <v>1</v>
       </c>
       <c r="D494" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E494" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F494" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G494" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H494" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="495" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14804,19 +14804,19 @@
         <v>1</v>
       </c>
       <c r="D495" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E495" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F495" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G495" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H495" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="496" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14830,19 +14830,19 @@
         <v>1</v>
       </c>
       <c r="D496" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E496" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F496" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G496" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H496" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="497" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14856,19 +14856,19 @@
         <v>1</v>
       </c>
       <c r="D497" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E497" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F497" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G497" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H497" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="498" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14882,19 +14882,19 @@
         <v>1</v>
       </c>
       <c r="D498" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E498" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F498" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G498" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H498" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="499" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14908,19 +14908,19 @@
         <v>1</v>
       </c>
       <c r="D499" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E499" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F499" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G499" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H499" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="500" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14934,19 +14934,19 @@
         <v>1</v>
       </c>
       <c r="D500" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E500" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F500" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G500" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H500" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="501" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14960,19 +14960,19 @@
         <v>1</v>
       </c>
       <c r="D501" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E501" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F501" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G501" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H501" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="502" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -14986,19 +14986,19 @@
         <v>1</v>
       </c>
       <c r="D502" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E502" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F502" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G502" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H502" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="503" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -15012,19 +15012,19 @@
         <v>1</v>
       </c>
       <c r="D503" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E503" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F503" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G503" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H503" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="504" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -15038,19 +15038,19 @@
         <v>1</v>
       </c>
       <c r="D504" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E504" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F504" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G504" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H504" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="505" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -15064,19 +15064,19 @@
         <v>1</v>
       </c>
       <c r="D505" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E505" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F505" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G505" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H505" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="506" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -15090,19 +15090,19 @@
         <v>1</v>
       </c>
       <c r="D506" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E506" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F506" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G506" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H506" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="507" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -15116,19 +15116,19 @@
         <v>1</v>
       </c>
       <c r="D507" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E507" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F507" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G507" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H507" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="508" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -15142,19 +15142,19 @@
         <v>1</v>
       </c>
       <c r="D508" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E508" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F508" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G508" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H508" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="509" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -15168,19 +15168,19 @@
         <v>1</v>
       </c>
       <c r="D509" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E509" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F509" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G509" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H509" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="510" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -15194,19 +15194,19 @@
         <v>1</v>
       </c>
       <c r="D510" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E510" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F510" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G510" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H510" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="511" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -15220,19 +15220,19 @@
         <v>1</v>
       </c>
       <c r="D511" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E511" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F511" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G511" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H511" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="512" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -15246,19 +15246,19 @@
         <v>1</v>
       </c>
       <c r="D512" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E512" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F512" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G512" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H512" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="513" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -15272,19 +15272,19 @@
         <v>1</v>
       </c>
       <c r="D513" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E513" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F513" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G513" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H513" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:sparkles: Did a lot of the data analysis.
</commit_message>
<xml_diff>
--- a/Documentation/Video Recording Progress.xlsx
+++ b/Documentation/Video Recording Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fcortevargas/Thesis/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A49AA9-03B4-4640-9440-5ECD27B63B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24BFC9A-1BC8-9444-8A72-7A5FC5B0CCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{E3E76E12-45DE-2C46-8A4D-60502D85C9C5}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{E3E76E12-45DE-2C46-8A4D-60502D85C9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1933,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95367985-2CDA-8742-AA4C-0FF0C0A9DC04}">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
-      <selection activeCell="C479" sqref="C479:H513"/>
+    <sheetView tabSelected="1" topLeftCell="A480" workbookViewId="0">
+      <selection activeCell="D418" sqref="D418:D513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>